<commit_message>
Last updates about seed.db
</commit_message>
<xml_diff>
--- a/db/kocgiri1.xlsx
+++ b/db/kocgiri1.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Koçgiri Hadisesine Ait Merkez Ordusu Kumandanlığının Cereyan Eden Muhaberat</t>
   </si>
   <si>
-    <t xml:space="preserve">14. Süvari Fırka Kumandanı Fahri, 29. Fırka Kumandanı Baki, Merkez Ordusu Kumandanı Nurettin, Nurettin Paşa, Merkez Ordusu Kumandanı Nurettin İbrahim Sakallı Nurettin, Merkez Ordusu Kumandanı Nureddin, Nureddin Paşa, Merkez Ordusu Kumandanı Nureddin İbrahim, Sakallı Nureddin, Erkan-ı Harbiye Umumiye Reisi Fevzi, Fevzi Çakmak, 14. Fırka Kumandanı Hayri, Erkan-ı Harbiye Reisi Hüseyin Hüsnü, Şark Cephesi Kumandanı Kazım Karabekir, Erkan-ı Harbiye Umumiye Reisi Vekili Fevzi, Süvari Liva Vekil-i Sani Mustafa,</t>
+    <t xml:space="preserve">14. Süvari Fırka Kumandanı Fahri</t>
   </si>
   <si>
     <t xml:space="preserve">Merkez Ordusu Kumandanlığı, Erkan-ı Harbiye Umumiye Riyaseti,  5. Fırka Kumandanlığı, Çorum Fırka Kumandanlığı, 15. Fırka Kumandanlığı, Yozgat Mıntıka Kumandanlığı, Sivas Liva Kumandanlığı, Amasya Mutasarrıflığı, Yozgat Mutasarrıflığı, Çorum Mutasarrıflığı, Tokat Mutasarrıflığı, Canik Mutasarrıflığı, Ordu Mutasarrıflığı, Sivas Vilayeti, Süvari Fırkası Kumandanlığı, </t>
@@ -1219,7 +1219,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1246,10 +1246,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1353,16 +1349,16 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="60"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="63.29"/>
@@ -1370,7 +1366,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="45.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2143,13 +2139,13 @@
       <c r="F27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2178,7 +2174,7 @@
       <c r="H28" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="I28" s="4" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2201,13 +2197,13 @@
       <c r="F29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>121</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="4" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2236,7 +2232,7 @@
       <c r="H30" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="4" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2578,7 +2574,7 @@
       <c r="F42" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G42" s="8" t="s">
         <v>175</v>
       </c>
       <c r="H42" s="4" t="s">
@@ -2634,7 +2630,7 @@
       <c r="F44" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="9" t="s">
         <v>182</v>
       </c>
       <c r="H44" s="4" t="s">
@@ -3069,7 +3065,7 @@
       <c r="F59" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="10" t="s">
         <v>238</v>
       </c>
       <c r="H59" s="4" t="s">
@@ -3368,12 +3364,12 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>